<commit_message>
Sprawdza czy uzytkownik poprawnie odpowiada
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kacper\Desktop\exp\Okregi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kacper\Desktop\Okregi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608ACF78-071F-4615-9ACE-729B444EE4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D736CD1-6800-4CA6-A229-36D70286097F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>User</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Timestamp</t>
+  </si>
+  <si>
+    <t>AnswerIsCorrect</t>
   </si>
 </sst>
 </file>
@@ -417,15 +420,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,20 +453,24 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G1 I1:J1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pozbywa sie pustych linii przy zapisie danych
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kacper\Desktop\Okregi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D736CD1-6800-4CA6-A229-36D70286097F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2339468A-F24E-4B99-BBEC-309AD9F57FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>User</t>
   </si>
@@ -40,7 +40,10 @@
     <t>UserAnswer</t>
   </si>
   <si>
-    <t>Timestamp</t>
+    <t>TimestampStart</t>
+  </si>
+  <si>
+    <t>TimestampEnd</t>
   </si>
   <si>
     <t>AnswerIsCorrect</t>
@@ -420,18 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="8" max="8" width="16" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,21 +456,18 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G1 I1:J1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:I1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>